<commit_message>
adds more functionality on the alamid framework
</commit_message>
<xml_diff>
--- a/source/sample data.xlsx
+++ b/source/sample data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve"> Robert A. Cruz --- Camiguin St., Aluba Subdv. CDOC</t>
   </si>
@@ -247,14 +247,34 @@
   </si>
   <si>
     <t>Repair Panel Indicators</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Labor Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -282,8 +302,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,306 +614,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="D10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="D16" t="s">
+    <row r="17" spans="1:4">
+      <c r="D17" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="D23" t="s">
+    <row r="24" spans="1:4">
+      <c r="D24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="D25" t="s">
+    <row r="26" spans="1:4">
+      <c r="D26" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>70</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="D34" t="s">
+    <row r="35" spans="1:4">
+      <c r="D35" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>